<commit_message>
Complete summary of statistics
</commit_message>
<xml_diff>
--- a/ana/Summary of Analysis.xlsx
+++ b/ana/Summary of Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Jenn\Documents\TwoRateProprioception\ana\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383EE85E-C4EB-42D5-87C2-BD5B0F3EEB66}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC37C287-8D55-4306-AC0F-A5ADDD5A89B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{EB8FF4AF-5815-4456-8224-0507E76FF27F}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="64">
   <si>
     <t>aligned</t>
   </si>
@@ -210,6 +210,18 @@
   </si>
   <si>
     <t>t(11.34) = -0.20, p = 0.85, d</t>
+  </si>
+  <si>
+    <t>No-Cursor VS No-Cursor -No- Cursors</t>
+  </si>
+  <si>
+    <t>F(3,120) = 106.74, p &lt; .001</t>
+  </si>
+  <si>
+    <t>F(1,40) = 3.01, p = 0.09</t>
+  </si>
+  <si>
+    <t>F(3,120) = 1.43, p = 0.239</t>
   </si>
 </sst>
 </file>
@@ -319,9 +331,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -355,6 +364,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -669,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F30A55-BAB0-4AF0-8398-2175355D4A86}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,179 +692,179 @@
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -860,59 +872,73 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="13" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>